<commit_message>
Update tasks.md: Document local persistence and frequent commit rules
</commit_message>
<xml_diff>
--- a/informacion fichas 3 modelado de datos.xlsx
+++ b/informacion fichas 3 modelado de datos.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Juan Vega\Fichas alcantarillado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A277638D-336D-44AE-9BBC-881211521522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D91342-9615-4883-B099-84A634157EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{5DBDE8C9-116B-489E-90E5-06C84F1DF031}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{5DBDE8C9-116B-489E-90E5-06C84F1DF031}"/>
   </bookViews>
   <sheets>
-    <sheet name="Pozo" sheetId="1" r:id="rId1"/>
-    <sheet name="Tuberias_entrada" sheetId="2" r:id="rId2"/>
-    <sheet name="Tuberias_salida" sheetId="3" r:id="rId3"/>
-    <sheet name="Sumideros" sheetId="4" r:id="rId4"/>
+    <sheet name="POZO" sheetId="1" r:id="rId1"/>
+    <sheet name="TUBERIAS" sheetId="2" r:id="rId2"/>
+    <sheet name="SUMIDEROS" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="80">
   <si>
     <t>Dirección</t>
   </si>
@@ -107,9 +106,6 @@
     <t>Tipo Cono</t>
   </si>
   <si>
-    <t>Materia Cono</t>
-  </si>
-  <si>
     <t>Estado Cono</t>
   </si>
   <si>
@@ -218,9 +214,6 @@
     <t>Emboquillado</t>
   </si>
   <si>
-    <t>Logitud</t>
-  </si>
-  <si>
     <t>PVC</t>
   </si>
   <si>
@@ -263,13 +256,28 @@
     <t>Vía</t>
   </si>
   <si>
-    <t>Materia Tuberia</t>
-  </si>
-  <si>
     <t>H salida (m)</t>
   </si>
   <si>
     <t>H llegada (m)</t>
+  </si>
+  <si>
+    <t>Material Cono</t>
+  </si>
+  <si>
+    <t>Longitud</t>
+  </si>
+  <si>
+    <t>Material Tuberia</t>
+  </si>
+  <si>
+    <t>tipo_tuberia</t>
+  </si>
+  <si>
+    <t>Entrada</t>
+  </si>
+  <si>
+    <t>Salida</t>
   </si>
 </sst>
 </file>
@@ -645,14 +653,14 @@
   <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -709,46 +717,46 @@
         <v>21</v>
       </c>
       <c r="T1" t="s">
+        <v>74</v>
+      </c>
+      <c r="U1" t="s">
         <v>22</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>23</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>24</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>25</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>26</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>27</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>28</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>29</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>30</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>31</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>32</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>33</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>34</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
@@ -768,76 +776,76 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
         <v>36</v>
-      </c>
-      <c r="G2" t="s">
-        <v>37</v>
       </c>
       <c r="K2">
         <v>13292</v>
       </c>
       <c r="L2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" t="s">
         <v>38</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>39</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>40</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>41</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" t="s">
         <v>43</v>
       </c>
-      <c r="R2" t="s">
-        <v>41</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>44</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" t="s">
         <v>45</v>
       </c>
-      <c r="U2" t="s">
-        <v>43</v>
-      </c>
-      <c r="V2" t="s">
-        <v>41</v>
-      </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y2" t="s">
         <v>46</v>
       </c>
-      <c r="X2" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>47</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>48</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>49</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD2" t="s">
         <v>50</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>51</v>
       </c>
       <c r="AE2">
         <v>0</v>
       </c>
       <c r="AF2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -847,84 +855,119 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D5E7137-8E15-46A0-9EFE-E43E05F35317}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>55</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>56</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
         <v>57</v>
       </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" t="s">
-        <v>59</v>
+      <c r="I1" t="s">
+        <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2">
         <v>300</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" t="s">
         <v>60</v>
       </c>
-      <c r="E2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" t="s">
-        <v>62</v>
-      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3">
+        <v>200</v>
+      </c>
+      <c r="E3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3">
+        <v>0.90569999999999995</v>
+      </c>
+      <c r="G3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4">
+        <v>200</v>
+      </c>
+      <c r="E4" t="s">
         <v>63</v>
       </c>
-      <c r="C3">
-        <v>200</v>
-      </c>
-      <c r="D3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3">
-        <v>0.90569999999999995</v>
-      </c>
-      <c r="F3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" t="s">
-        <v>62</v>
+      <c r="F4">
+        <v>0.96160000000000001</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -933,39 +976,39 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7482126D-BB8E-4DC9-8DCD-E37FB28D1299}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CD0B5E4-E54F-420F-BBA3-B33F66A051DA}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" t="s">
-        <v>57</v>
-      </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="G1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="H1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -973,83 +1016,19 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2">
-        <v>200</v>
-      </c>
-      <c r="D2" t="s">
         <v>65</v>
-      </c>
-      <c r="E2">
-        <v>0.96160000000000001</v>
-      </c>
-      <c r="F2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CD0B5E4-E54F-420F-BBA3-B33F66A051DA}">
-  <dimension ref="A1:H5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>67</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E2">
         <v>150</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G2">
         <v>0.69</v>
@@ -1063,19 +1042,19 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E3">
         <v>150</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G3">
         <v>0.65</v>
@@ -1089,19 +1068,19 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E4">
         <v>150</v>
       </c>
       <c r="F4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G4">
         <v>0.55000000000000004</v>
@@ -1115,19 +1094,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E5">
         <v>150</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G5">
         <v>0.61</v>

</xml_diff>